<commit_message>
0.02.10 - Add check groups for steel members
</commit_message>
<xml_diff>
--- a/Source/Excel/Small_Model/Members.xlsx
+++ b/Source/Excel/Small_Model/Members.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aleksei\Havings\Code\demo.local\Source\Excel\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aleksei\Havings\Code\demo.local\Source\Excel\Small_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>GOST 26020</t>
   </si>
@@ -53,12 +53,6 @@
     <t>000011</t>
   </si>
   <si>
-    <t>betaAngle</t>
-  </si>
-  <si>
-    <t>sectionName</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -71,36 +65,6 @@
     <t>Beams GL+5000</t>
   </si>
   <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>z1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>z2</t>
-  </si>
-  <si>
-    <t>pin1</t>
-  </si>
-  <si>
-    <t>pin2</t>
-  </si>
-  <si>
-    <t>sectionType</t>
-  </si>
-  <si>
-    <t>isDivided</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -128,7 +92,67 @@
     <t>000001</t>
   </si>
   <si>
-    <t>B1</t>
+    <t>x1*</t>
+  </si>
+  <si>
+    <t>y1*</t>
+  </si>
+  <si>
+    <t>z1*</t>
+  </si>
+  <si>
+    <t>pin1*</t>
+  </si>
+  <si>
+    <t>sectionType*</t>
+  </si>
+  <si>
+    <t>sectionName*</t>
+  </si>
+  <si>
+    <t>betaAngle*</t>
+  </si>
+  <si>
+    <t>isDivided*</t>
+  </si>
+  <si>
+    <t>pin2*</t>
+  </si>
+  <si>
+    <t>x2*</t>
+  </si>
+  <si>
+    <t>y2*</t>
+  </si>
+  <si>
+    <t>z2*</t>
+  </si>
+  <si>
+    <t>C255</t>
+  </si>
+  <si>
+    <t>steel*</t>
+  </si>
+  <si>
+    <t>Ry*</t>
+  </si>
+  <si>
+    <t>gammaC*</t>
+  </si>
+  <si>
+    <t>muXZ*</t>
+  </si>
+  <si>
+    <t>muXY*</t>
+  </si>
+  <si>
+    <t>FC*</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Балка 1</t>
   </si>
 </sst>
 </file>
@@ -521,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,61 +557,81 @@
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="4"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="9.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
@@ -599,10 +643,12 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -640,10 +686,28 @@
       <c r="M3" s="1">
         <v>5</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="6">
+        <v>240</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>120</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -681,10 +745,28 @@
       <c r="M4" s="1">
         <v>5</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="6">
+        <v>240</v>
+      </c>
+      <c r="P4" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>125</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -722,10 +804,28 @@
       <c r="M5" s="1">
         <v>5</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="6">
+        <v>240</v>
+      </c>
+      <c r="P5" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>3</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3</v>
+      </c>
+      <c r="S5" s="1">
+        <v>130</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -763,18 +863,36 @@
       <c r="M6" s="1">
         <v>10</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="6">
+        <v>240</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4</v>
+      </c>
+      <c r="S6" s="1">
+        <v>135</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -801,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1">
         <v>5</v>
@@ -812,10 +930,28 @@
       <c r="M8" s="1">
         <v>5</v>
       </c>
+      <c r="N8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="6">
+        <v>240</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="S8" s="1">
+        <v>400</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -842,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
@@ -853,18 +989,36 @@
       <c r="M9" s="1">
         <v>5</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="6">
+        <v>240</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="S9" s="1">
+        <v>400</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -902,10 +1056,28 @@
       <c r="M11" s="1">
         <v>5</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="6">
+        <v>240</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="S11" s="1">
+        <v>200</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -942,6 +1114,24 @@
       </c>
       <c r="M12" s="1">
         <v>5</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="6">
+        <v>240</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="S12" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>